<commit_message>
business overview export 1/3 done
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Journal Report" sheetId="1" r:id="rId1"/>
+    <sheet name="Trail Balance" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -383,85 +383,31 @@
     <col min="1" max="1" width="50.83203125" customWidth="1"/>
     <col min="2" max="2" width="50.83203125" customWidth="1"/>
     <col min="3" max="3" width="50.83203125" customWidth="1"/>
+    <col min="4" max="4" width="50.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ElHadar-PLC - Journal Report - From Thu Dec 12 2019 to Tue Dec 12 2023</v>
+        <v>ElHadar-PLC  Statement of profit or Loss and other comprehensive income  From Fri Jan 01 1999 To Sun Jan 01 2023</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>WED AUG 19 2020 - JOURNAL - CS/DS/MT/013</v>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Account</v>
       </c>
-      <c r="B6" t="str">
-        <v>Debit</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Credit</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>WED AUG 19 2020 - JOURNAL</v>
-      </c>
-      <c r="B8" t="str">
-        <v>DEBIT</v>
-      </c>
-      <c r="C8" t="str">
-        <v>CREDIT</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="str">
+      <c r="B4" t="str">
         <v/>
       </c>
-      <c r="B9" t="str">
-        <v>0</v>
-      </c>
-      <c r="C9" t="str">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v>WED AUG 19 2020 - JOURNAL - PR-0</v>
-      </c>
-      <c r="B12" t="str">
-        <v>Debit</v>
-      </c>
-      <c r="C12" t="str">
-        <v>Credit</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="str">
-        <v>WED AUG 19 2020 - JOURNAL</v>
-      </c>
-      <c r="B14" t="str">
-        <v>DEBIT</v>
-      </c>
-      <c r="C14" t="str">
-        <v>CREDIT</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="str">
-        <v/>
-      </c>
-      <c r="B15" t="str">
-        <v>0</v>
-      </c>
-      <c r="C15" t="str">
-        <v>12</v>
+      <c r="C4" t="str">
+        <v>Total</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:C3"/>
+    <mergeCell ref="A1:D3"/>
   </mergeCells>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C15"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished business overview exports
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -388,26 +388,63 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ElHadar-PLC  Statement of profit or Loss and other comprehensive income  From Fri Jan 01 1999 To Sun Jan 01 2023</v>
+        <v>ElHadar-PLC  Statement of cash flow  From Fri Jan 01 1999 To Sat Jan 01 2022</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v>Account</v>
+        <v/>
       </c>
       <c r="B4" t="str">
-        <v/>
+        <v>Account Code</v>
       </c>
       <c r="C4" t="str">
         <v>Total</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v/>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Beginning Cash Balance</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>IDK</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v xml:space="preserve"> HELLO(HELLO)</v>
+      </c>
+      <c r="B10" t="str">
+        <v/>
+      </c>
+      <c r="C10" t="str">
+        <v>-988</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v/>
+      </c>
+      <c r="B12" t="str">
+        <v/>
+      </c>
+      <c r="C12" t="str">
+        <v>-988</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D3"/>
+    <mergeCell ref="A1:C3"/>
   </mergeCells>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:C12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
finished up general exports, and fixed schema
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Trail Balance" sheetId="1" r:id="rId1"/>
+    <sheet name="exportReadyJournal" sheetId="1" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
@@ -375,76 +375,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="50.83203125" customWidth="1"/>
-    <col min="2" max="2" width="50.83203125" customWidth="1"/>
-    <col min="3" max="3" width="50.83203125" customWidth="1"/>
-    <col min="4" max="4" width="50.83203125" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" customWidth="1"/>
+    <col min="2" max="2" width="27.83203125" customWidth="1"/>
+    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
+    <col min="8" max="8" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="18.83203125" customWidth="1"/>
+    <col min="10" max="10" width="17.83203125" customWidth="1"/>
+    <col min="11" max="11" width="18.83203125" customWidth="1"/>
+    <col min="12" max="12" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="16.83203125" customWidth="1"/>
+    <col min="14" max="14" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>ElHadar-PLC  Statement of cash flow  From Fri Jan 01 1999 To Sat Jan 01 2022</v>
+        <v>report_basis</v>
+      </c>
+      <c r="B1" t="str">
+        <v>journal_posting_status</v>
+      </c>
+      <c r="C1" t="str">
+        <v>journal_type</v>
+      </c>
+      <c r="D1" t="str">
+        <v>reference_number</v>
+      </c>
+      <c r="E1" t="str">
+        <v>is_inclusive_tax</v>
+      </c>
+      <c r="F1" t="str">
+        <v>tax_name</v>
+      </c>
+      <c r="G1" t="str">
+        <v>tax_percentage</v>
+      </c>
+      <c r="H1" t="str">
+        <v>tax_type</v>
+      </c>
+      <c r="I1" t="str">
+        <v>amount_credit</v>
+      </c>
+      <c r="J1" t="str">
+        <v>account_name</v>
+      </c>
+      <c r="K1" t="str">
+        <v>currency_code</v>
+      </c>
+      <c r="L1" t="str">
+        <v>total</v>
+      </c>
+      <c r="M1" t="str">
+        <v>description</v>
+      </c>
+      <c r="N1" t="str">
+        <v>journal_date</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="str">
+        <v>accrual</v>
+      </c>
+      <c r="B2" t="str">
+        <v>POSTED</v>
+      </c>
+      <c r="E2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="str">
+        <v>a</v>
+      </c>
+      <c r="K2" t="str">
+        <v>ETB</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="N2" t="str">
+        <v>Wed Aug 19 2020</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>accrual</v>
+      </c>
+      <c r="B3" t="str">
+        <v>POSTED</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="str">
+        <v>IDK</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3" t="str">
+        <v>compound_tax</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3" t="str">
+        <v>HELLO</v>
+      </c>
+      <c r="K3" t="str">
+        <v>ETB</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="M3" t="str">
+        <v>Hello</v>
+      </c>
+      <c r="N3" t="str">
+        <v>Wed Aug 19 2020</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="str">
-        <v/>
+        <v>accrual</v>
       </c>
       <c r="B4" t="str">
-        <v>Account Code</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Total</v>
+        <v>POSTED</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="str">
+        <v>a</v>
+      </c>
+      <c r="K4" t="str">
+        <v>ETB</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="N4" t="str">
+        <v>Wed Aug 19 2020</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="str">
-        <v/>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>Beginning Cash Balance</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="str">
-        <v>IDK</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="str">
-        <v xml:space="preserve"> HELLO(HELLO)</v>
-      </c>
-      <c r="B10" t="str">
-        <v/>
-      </c>
-      <c r="C10" t="str">
-        <v>-988</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="str">
-        <v/>
-      </c>
-      <c r="B12" t="str">
-        <v/>
-      </c>
-      <c r="C12" t="str">
-        <v>-988</v>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="str">
+        <v>a</v>
+      </c>
+      <c r="K5" t="str">
+        <v>ETB</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="N5" t="str">
+        <v>Thu Aug 20 2020</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:C3"/>
-  </mergeCells>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C12"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>